<commit_message>
rearrange main post-process routine
</commit_message>
<xml_diff>
--- a/R script overhaul checklist.xlsx
+++ b/R script overhaul checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Joe_Proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.caracappa\Documents\GitHub\neus-atlantis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -948,11 +948,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>